<commit_message>
Actualizar precios con datos nuevos
</commit_message>
<xml_diff>
--- a/precios_creatina.xlsx
+++ b/precios_creatina.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45804.48548514055</v>
+        <v>45804.48548513889</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -474,6 +474,26 @@
         </is>
       </c>
       <c r="D2" t="inlineStr">
+        <is>
+          <t>12,88€</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45804.43437102554</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>12,88€</t>
         </is>

</xml_diff>

<commit_message>
añadido funcionalidad de envio por correo
</commit_message>
<xml_diff>
--- a/precios_creatina.xlsx
+++ b/precios_creatina.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -781,7 +781,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45818.39375911181</v>
+        <v>45818.3937591088</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -794,6 +794,386 @@
         </is>
       </c>
       <c r="D18" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45833.41288174769</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>45833.41722056713</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>45833.41746144676</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>45833.41859150463</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45833.42342791666</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45833.42990267361</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>45833.43051061343</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45833.43422083333</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45833.4369330787</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>45833.43815046296</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>45833.43892174769</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>45833.43977028935</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45833.44140856482</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>45833.44283475694</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>45833.44410322917</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>45833.44530853009</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>45833.45332490741</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>45833.45424282407</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>45833.45891689683</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
         <is>
           <t>15,41€</t>
         </is>

</xml_diff>

<commit_message>
Mejorar sistema de correos con alertas de precios históricos
- Añadida función analizar_precio_historico() para detectar precios máximos y mínimos
- Mejorado formato de correo con versión HTML y texto plano
- Agregados emojis y mensajes destacados para precios récord
- Solucionado problema de texto oculto en Gmail
- Actualizada estructura de correo para mejor compatibilidad

Características:
🎉 Alerta cuando es el precio más bajo histórico
⚠️ Alerta cuando es el precio más alto histórico
📧 Formato dual HTML/texto para mejor visualización
</commit_message>
<xml_diff>
--- a/precios_creatina.xlsx
+++ b/precios_creatina.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45833.45891689683</v>
+        <v>45833.45891689815</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1174,6 +1174,126 @@
         </is>
       </c>
       <c r="D37" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>45834.45434878472</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>12,88€</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>45853.38054951389</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>45853.38514180556</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>45853.38685481482</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45853.39298033565</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>15,41€</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>45853.39427826957</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>CREATINA MONOHIDRATO EN POLVO</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>1Kg</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
         <is>
           <t>15,41€</t>
         </is>

</xml_diff>